<commit_message>
up bao cao tuan 9 - 10
</commit_message>
<xml_diff>
--- a/Báo Cáo Tuần 8/BaoCaoCongViecT8.xlsx
+++ b/Báo Cáo Tuần 8/BaoCaoCongViecT8.xlsx
@@ -234,52 +234,16 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -294,18 +258,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,6 +268,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -601,7 +601,7 @@
   <dimension ref="B1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E16"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,305 +614,335 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="14"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="28"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="21" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="21" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="21" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="22"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="21" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="21" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="21" t="s">
+      <c r="I11" s="2"/>
+      <c r="J11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="24"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="21" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="21" t="s">
+      <c r="G13" s="2"/>
+      <c r="H13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="21" t="s">
+      <c r="I13" s="2"/>
+      <c r="J13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="25" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="20"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="22"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="22"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="24"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="H9:I10"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="J11:K12"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="H5:I6"/>
+    <mergeCell ref="H7:I8"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="D1:K2"/>
+    <mergeCell ref="B1:C4"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:G4"/>
     <mergeCell ref="J13:K14"/>
     <mergeCell ref="J17:K18"/>
     <mergeCell ref="J19:K20"/>
@@ -929,36 +959,6 @@
     <mergeCell ref="H19:I20"/>
     <mergeCell ref="B13:C14"/>
     <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="D17:E18"/>
-    <mergeCell ref="D19:E20"/>
-    <mergeCell ref="D1:K2"/>
-    <mergeCell ref="B1:C4"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="B5:C6"/>
-    <mergeCell ref="H5:I6"/>
-    <mergeCell ref="H7:I8"/>
-    <mergeCell ref="H9:I10"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="J9:K10"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="J11:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>